<commit_message>
modificato comportamento caricamento massivo per compilare UO II LIVELLO
</commit_message>
<xml_diff>
--- a/pages/templates/utenti_template.xlsx
+++ b/pages/templates/utenti_template.xlsx
@@ -125,7 +125,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
@@ -647,8 +648,8 @@
     <col customWidth="1" min="4" max="4" width="15.421875"/>
     <col customWidth="1" min="8" max="8" width="22.8515625"/>
     <col customWidth="1" min="9" max="9" width="24.421875"/>
-    <col customWidth="1" min="10" max="10" width="22.421875"/>
-    <col customWidth="1" min="11" max="11" width="17.00390625"/>
+    <col customWidth="1" min="10" max="11" width="22.421875"/>
+    <col customWidth="1" min="12" max="12" width="17.00390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -682,12 +683,15 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
@@ -696,7 +700,7 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>29221</v>
       </c>
       <c r="E2" t="s">
@@ -711,13 +715,14 @@
       <c r="H2">
         <v>3481234567</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1"/>
+      <c r="L2">
         <v>12345</v>
       </c>
     </row>
@@ -731,7 +736,7 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>31080</v>
       </c>
       <c r="E3" t="s">
@@ -746,12 +751,13 @@
       <c r="H3">
         <v>3331234567</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" ht="14.25"/>
   </sheetData>

</xml_diff>